<commit_message>
correccion 162 por 166
</commit_message>
<xml_diff>
--- a/preguntas/RevisionPreguntasDeExamen.xlsx
+++ b/preguntas/RevisionPreguntasDeExamen.xlsx
@@ -456,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -491,20 +491,12 @@
     <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -806,7 +798,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -834,7 +826,7 @@
     <row r="2" spans="1:19">
       <c r="A2">
         <f ca="1">ROUND((RAND()*17),2)</f>
-        <v>3.88</v>
+        <v>2.39</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -894,7 +886,7 @@
     <row r="3" spans="1:19">
       <c r="A3">
         <f t="shared" ref="A3:A16" ca="1" si="0">ROUND((RAND()*17),2)</f>
-        <v>2.62</v>
+        <v>2.29</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -954,7 +946,7 @@
     <row r="4" spans="1:19">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>4.25</v>
+        <v>10.58</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -1014,7 +1006,7 @@
     <row r="5" spans="1:19">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>13.67</v>
+        <v>10.99</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
@@ -1072,7 +1064,7 @@
     <row r="6" spans="1:19">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
-        <v>4.8899999999999997</v>
+        <v>7.9</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
@@ -1132,7 +1124,7 @@
     <row r="7" spans="1:19">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>5.65</v>
+        <v>9.5500000000000007</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
@@ -1192,7 +1184,7 @@
     <row r="8" spans="1:19">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>3.63</v>
+        <v>7.9</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -1252,7 +1244,7 @@
     <row r="9" spans="1:19">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.55</v>
+        <v>7.46</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>14</v>
@@ -1310,7 +1302,7 @@
     <row r="10" spans="1:19">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85</v>
+        <v>2.71</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>14</v>
@@ -1368,7 +1360,7 @@
     <row r="11" spans="1:19">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>9.73</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>15</v>
@@ -1426,7 +1418,7 @@
     <row r="12" spans="1:19">
       <c r="A12">
         <f t="shared" ca="1" si="0"/>
-        <v>15.68</v>
+        <v>14.87</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>8</v>
@@ -1484,7 +1476,7 @@
     <row r="13" spans="1:19">
       <c r="A13">
         <f t="shared" ca="1" si="0"/>
-        <v>10.58</v>
+        <v>16.29</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>9</v>
@@ -1542,7 +1534,7 @@
     <row r="14" spans="1:19">
       <c r="A14">
         <f t="shared" ca="1" si="0"/>
-        <v>7.61</v>
+        <v>3.59</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>12</v>
@@ -1602,7 +1594,7 @@
     <row r="15" spans="1:19">
       <c r="A15">
         <f t="shared" ca="1" si="0"/>
-        <v>10.27</v>
+        <v>7.92</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>10</v>
@@ -1662,7 +1654,7 @@
     <row r="16" spans="1:19">
       <c r="A16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.39</v>
+        <v>14.83</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>0</v>
@@ -2076,11 +2068,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2106,7 +2097,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1">
+    <row r="2" spans="1:8">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -2117,7 +2108,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2128,7 +2119,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1">
+    <row r="4" spans="1:8">
       <c r="A4" s="16">
         <v>1</v>
       </c>
@@ -2139,7 +2130,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1">
+    <row r="5" spans="1:8">
       <c r="A5" s="16">
         <v>1</v>
       </c>
@@ -2150,7 +2141,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1">
+    <row r="6" spans="1:8">
       <c r="A6" s="16">
         <v>1</v>
       </c>
@@ -2161,7 +2152,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1">
+    <row r="7" spans="1:8">
       <c r="A7" s="16">
         <v>1</v>
       </c>
@@ -2181,7 +2172,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1">
+    <row r="8" spans="1:8">
       <c r="A8" s="6">
         <v>1</v>
       </c>
@@ -2198,7 +2189,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1">
+    <row r="9" spans="1:8">
       <c r="A9" s="6">
         <v>1</v>
       </c>
@@ -2209,8 +2200,10 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="6" customFormat="1" ht="27" hidden="1" customHeight="1">
-      <c r="A10" s="16"/>
+    <row r="10" spans="1:8" s="6" customFormat="1" ht="27" customHeight="1">
+      <c r="A10" s="16">
+        <v>1</v>
+      </c>
       <c r="B10" s="14">
         <v>69</v>
       </c>
@@ -2220,8 +2213,10 @@
       </c>
       <c r="E10"/>
     </row>
-    <row r="11" spans="1:8" hidden="1">
-      <c r="A11" s="16"/>
+    <row r="11" spans="1:8">
+      <c r="A11" s="16">
+        <v>1</v>
+      </c>
       <c r="B11" s="14">
         <v>72</v>
       </c>
@@ -2229,7 +2224,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1">
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2244,7 +2239,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1">
+    <row r="13" spans="1:8">
       <c r="A13" s="16"/>
       <c r="B13" s="12">
         <v>74</v>
@@ -2253,7 +2248,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1">
+    <row r="14" spans="1:8">
       <c r="A14" s="16">
         <v>1</v>
       </c>
@@ -2264,7 +2259,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1">
+    <row r="15" spans="1:8">
       <c r="A15" s="16">
         <v>1</v>
       </c>
@@ -2275,7 +2270,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1">
+    <row r="16" spans="1:8">
       <c r="A16" s="6">
         <v>1</v>
       </c>
@@ -2286,7 +2281,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:17" s="6" customFormat="1" hidden="1">
+    <row r="17" spans="1:17" s="6" customFormat="1">
       <c r="A17" s="6">
         <v>1</v>
       </c>
@@ -2300,6 +2295,9 @@
       <c r="E17"/>
     </row>
     <row r="18" spans="1:17">
+      <c r="A18" s="16">
+        <v>1</v>
+      </c>
       <c r="B18" s="6">
         <v>121</v>
       </c>
@@ -2311,7 +2309,9 @@
       </c>
     </row>
     <row r="19" spans="1:17">
-      <c r="A19" s="6"/>
+      <c r="A19" s="6">
+        <v>1</v>
+      </c>
       <c r="B19" s="11">
         <v>125</v>
       </c>
@@ -2334,8 +2334,10 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="3"/>
     </row>
-    <row r="20" spans="1:17" hidden="1">
-      <c r="A20" s="16"/>
+    <row r="20" spans="1:17">
+      <c r="A20" s="22">
+        <v>1</v>
+      </c>
       <c r="B20" s="14">
         <v>127</v>
       </c>
@@ -2343,8 +2345,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:17" hidden="1">
-      <c r="A21" s="16"/>
+    <row r="21" spans="1:17">
+      <c r="A21" s="22">
+        <v>1</v>
+      </c>
       <c r="B21" s="14">
         <v>139</v>
       </c>
@@ -2352,7 +2356,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:17" hidden="1">
+    <row r="22" spans="1:17">
       <c r="A22" s="16">
         <v>1</v>
       </c>
@@ -2363,17 +2367,27 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:17" hidden="1">
-      <c r="A23" s="16"/>
+    <row r="23" spans="1:17">
+      <c r="A23" s="22">
+        <v>1</v>
+      </c>
       <c r="B23" s="14">
         <v>161</v>
       </c>
       <c r="D23" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" hidden="1">
-      <c r="A24" s="16"/>
+      <c r="G23">
+        <v>162</v>
+      </c>
+      <c r="H23">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="A24" s="22">
+        <v>1</v>
+      </c>
       <c r="B24" s="14">
         <v>165</v>
       </c>
@@ -2381,7 +2395,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:17" hidden="1">
+    <row r="25" spans="1:17">
       <c r="A25" s="16">
         <v>1</v>
       </c>
@@ -2392,7 +2406,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:17" hidden="1">
+    <row r="26" spans="1:17">
       <c r="A26" s="6">
         <v>1</v>
       </c>
@@ -2403,7 +2417,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:17" hidden="1">
+    <row r="27" spans="1:17">
       <c r="A27" s="6">
         <v>1</v>
       </c>
@@ -2414,7 +2428,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:17" hidden="1">
+    <row r="28" spans="1:17">
       <c r="A28" s="18">
         <v>1</v>
       </c>
@@ -2425,7 +2439,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:17" hidden="1">
+    <row r="29" spans="1:17">
       <c r="A29" s="6">
         <v>1</v>
       </c>
@@ -2436,8 +2450,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:17" hidden="1">
-      <c r="A30" s="16"/>
+    <row r="30" spans="1:17">
+      <c r="A30" s="6">
+        <v>1</v>
+      </c>
       <c r="B30" s="12">
         <v>171</v>
       </c>
@@ -2446,7 +2462,7 @@
       </c>
       <c r="E30" s="16"/>
     </row>
-    <row r="31" spans="1:17" hidden="1">
+    <row r="31" spans="1:17">
       <c r="A31" s="16">
         <v>1</v>
       </c>
@@ -2457,7 +2473,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:17" hidden="1">
+    <row r="32" spans="1:17">
       <c r="A32" s="16">
         <v>1</v>
       </c>
@@ -2468,7 +2484,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:19" hidden="1">
+    <row r="33" spans="1:19">
       <c r="A33" s="16">
         <v>1</v>
       </c>
@@ -2479,7 +2495,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:19" hidden="1">
+    <row r="34" spans="1:19">
       <c r="A34" s="6">
         <v>1</v>
       </c>
@@ -2490,7 +2506,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:19" hidden="1">
+    <row r="35" spans="1:19">
       <c r="A35" s="6">
         <v>1</v>
       </c>
@@ -2501,7 +2517,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="1:19" hidden="1">
+    <row r="36" spans="1:19">
       <c r="A36" s="6">
         <v>1</v>
       </c>
@@ -2513,7 +2529,9 @@
       </c>
     </row>
     <row r="37" spans="1:19">
-      <c r="A37" s="6"/>
+      <c r="A37" s="6">
+        <v>1</v>
+      </c>
       <c r="B37" s="6">
         <v>194</v>
       </c>
@@ -2546,7 +2564,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:19" hidden="1">
+    <row r="39" spans="1:19">
       <c r="A39" s="6">
         <v>1</v>
       </c>
@@ -2557,8 +2575,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:19" hidden="1">
-      <c r="A40" s="16"/>
+    <row r="40" spans="1:19">
+      <c r="A40" s="6">
+        <v>1</v>
+      </c>
       <c r="B40" s="14">
         <v>234</v>
       </c>
@@ -2567,7 +2587,9 @@
       </c>
     </row>
     <row r="41" spans="1:19">
-      <c r="A41" s="6"/>
+      <c r="A41" s="6">
+        <v>1</v>
+      </c>
       <c r="B41" s="6">
         <v>237</v>
       </c>
@@ -2575,8 +2597,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="42" spans="1:19" hidden="1">
-      <c r="A42" s="16"/>
+    <row r="42" spans="1:19">
+      <c r="A42" s="6">
+        <v>1</v>
+      </c>
       <c r="B42" s="14">
         <v>240</v>
       </c>
@@ -2593,7 +2617,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:19" hidden="1">
+    <row r="44" spans="1:19">
       <c r="A44">
         <v>1</v>
       </c>
@@ -2608,7 +2632,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:19" hidden="1">
+    <row r="45" spans="1:19">
       <c r="A45" s="16">
         <v>1</v>
       </c>
@@ -2619,7 +2643,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:19" hidden="1">
+    <row r="46" spans="1:19">
       <c r="A46" s="6">
         <v>1</v>
       </c>
@@ -2630,7 +2654,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="47" spans="1:19" hidden="1">
+    <row r="47" spans="1:19">
       <c r="A47">
         <v>1</v>
       </c>
@@ -2645,7 +2669,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="48" spans="1:19" hidden="1">
+    <row r="48" spans="1:19">
       <c r="A48" s="16"/>
       <c r="B48" s="14">
         <v>258</v>
@@ -2654,7 +2678,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1">
+    <row r="49" spans="1:7">
       <c r="A49" s="16"/>
       <c r="B49" s="14">
         <v>274</v>
@@ -2663,7 +2687,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1">
+    <row r="50" spans="1:7">
       <c r="A50" s="16"/>
       <c r="B50" s="14">
         <v>279</v>
@@ -2672,7 +2696,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1">
+    <row r="51" spans="1:7">
       <c r="A51" s="18">
         <v>1</v>
       </c>
@@ -2683,23 +2707,23 @@
         <v>34</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1">
+    <row r="52" spans="1:7">
       <c r="A52">
         <f>SUM(A2:A51)</f>
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="B52">
         <v>50</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1">
+    <row r="53" spans="1:7">
       <c r="B53">
         <f>COUNT(B2:B51)-A52</f>
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C53">
         <f>COUNT(A2:A51)</f>
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="15" customHeight="1">
@@ -2803,12 +2827,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:B53">
-    <filterColumn colId="0">
-      <filters blank="1"/>
-    </filterColumn>
-    <filterColumn colId="1">
-      <colorFilter dxfId="0"/>
-    </filterColumn>
+    <filterColumn colId="0"/>
+    <filterColumn colId="1"/>
   </autoFilter>
   <sortState ref="B1:E52">
     <sortCondition ref="B1:B52"/>

</xml_diff>